<commit_message>
Xây dựng form GUI_QLDichVu và chỉnh sửa QLDatPhong
</commit_message>
<xml_diff>
--- a/DoAnQLKhachSan/GUI/HoaDon1.xlsx
+++ b/DoAnQLKhachSan/GUI/HoaDon1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DNT\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Desktop\DA_LTCSHARP2_05\SOURCE\DoAnQLKhachSan\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C184ACF4-4037-42F1-9830-4F678E5BD3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF75A49D-8CA3-401F-8AF7-E07039FE02EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{08E532CE-F582-4522-822B-F96A5A66C14B}"/>
   </bookViews>
@@ -83,19 +83,19 @@
     <t>STT</t>
   </si>
   <si>
-    <t>%HoaDon2.GiaPhong</t>
-  </si>
-  <si>
-    <t>%HoaDon2.SoNgay</t>
-  </si>
-  <si>
-    <t>%HoaDon2.TongTien</t>
-  </si>
-  <si>
-    <t>%HoaDon2.TenPhong</t>
-  </si>
-  <si>
-    <t>%HoaDon2.STT;insert:copystyles</t>
+    <t>%HoaDon1.STT;insert:copystyles</t>
+  </si>
+  <si>
+    <t>%HoaDon1.TenPhong</t>
+  </si>
+  <si>
+    <t>%HoaDon1.GiaPhong</t>
+  </si>
+  <si>
+    <t>%HoaDon1.SoNgay</t>
+  </si>
+  <si>
+    <t>%HoaDon1.TongTien</t>
   </si>
 </sst>
 </file>
@@ -256,7 +256,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -321,7 +321,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -620,7 +620,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,19 +778,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>19</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="G15" s="2"/>
     </row>

</xml_diff>